<commit_message>
Abbildungen für Kapitel 6+ Änderungen an Kap 6
</commit_message>
<xml_diff>
--- a/40_Messung/Projektarbeit_WS_18_19/C_mu_50erWellen.xlsx
+++ b/40_Messung/Projektarbeit_WS_18_19/C_mu_50erWellen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>C_mu</t>
   </si>
@@ -28,6 +28,18 @@
   </si>
   <si>
     <t>&lt;u_jet&gt;</t>
+  </si>
+  <si>
+    <t>Werte für 0rpm</t>
+  </si>
+  <si>
+    <t>Werte für rpm &gt;0</t>
+  </si>
+  <si>
+    <t>Größerer Druck nicht möglich, da sonst inkompressibel</t>
+  </si>
+  <si>
+    <t>pPlenum offen mittel</t>
   </si>
 </sst>
 </file>
@@ -345,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -356,7 +368,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -366,41 +378,138 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.16</v>
       </c>
       <c r="C3">
-        <f>(A3 *0.5*15^2*0.0205*1.2)/(2*0.384*0.159*10^(-3))</f>
-        <v>3626.1792452830182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>(A3*0.5*14.94^2*0.39*0.0534*1.17)/(2*0.384*0.19*10^(-3))</f>
+        <v>2981.7284337236847</v>
+      </c>
+      <c r="G3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H3">
+        <f>(G3*0.5*14.94^2*0.39*0.0534*1.17)/(2*0.384*0.19*10^(-3))</f>
+        <v>1192.6913734894738</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.32</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C6" si="0">(A4 *0.5*15^2*0.0205*1.2)/(2*0.384*0.159*10^(-3))</f>
-        <v>7252.3584905660364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C4:C6" si="0">(A4*0.5*14.94^2*0.39*0.0534*1.17)/(2*0.384*0.19*10^(-3))</f>
+        <v>5963.4568674473694</v>
+      </c>
+      <c r="G4">
+        <v>0.27</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="1">(G4*0.5*14.94^2*0.39*0.0534*1.17)/(2*0.384*0.19*10^(-3))</f>
+        <v>5031.6667319087182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.48</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>10878.537735849055</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8945.1853011710537</v>
+      </c>
+      <c r="G5">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>7752.4939276815803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.69</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>15637.897995283018</v>
+        <v>12858.703870433388</v>
+      </c>
+      <c r="G6">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>10846.037177669903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>(H8*2*0.384*0.00019)/(0.5*14.94^2*0.39*0.0534*1.17)</f>
+        <v>9.6588273010609446E-2</v>
+      </c>
+      <c r="H8">
+        <v>1800</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" ref="G9:G11" si="2">(H9*2*0.384*0.00019)/(0.5*14.94^2*0.39*0.0534*1.17)</f>
+        <v>0.24147068252652354</v>
+      </c>
+      <c r="H9">
+        <v>4500</v>
+      </c>
+      <c r="I9">
+        <v>2000</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.28976481903182827</v>
+      </c>
+      <c r="H10">
+        <v>5400</v>
+      </c>
+      <c r="I10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.32732692520262086</v>
+      </c>
+      <c r="H11">
+        <v>6100</v>
+      </c>
+      <c r="I11">
+        <v>4000</v>
+      </c>
+      <c r="J11">
+        <v>9000</v>
+      </c>
+      <c r="K11">
+        <f>SQRT(2*J11/1.17)</f>
+        <v>124.03473458920845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>